<commit_message>
close positions report prepared
</commit_message>
<xml_diff>
--- a/etc/Portfolio.Events.xlsx
+++ b/etc/Portfolio.Events.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -60,9 +60,6 @@
     <t>some text</t>
   </si>
   <si>
-    <t>US123456789</t>
-  </si>
-  <si>
     <t>GB001100110</t>
   </si>
   <si>
@@ -82,12 +79,24 @@
   </si>
   <si>
     <t>ignored</t>
+  </si>
+  <si>
+    <t>US111222333</t>
+  </si>
+  <si>
+    <t>DE777000011</t>
+  </si>
+  <si>
+    <t>Paul AG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -130,11 +139,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,11 +445,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E11"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +458,9 @@
     <col min="2" max="2" width="12.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" style="2" customWidth="1"/>
-    <col min="5" max="7" width="9.140625" style="2"/>
+    <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="6" max="6" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" style="2" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
@@ -462,10 +473,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -487,23 +498,23 @@
       <c r="B2" s="3">
         <v>41640</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="7">
+      <c r="C2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="5">
         <v>1</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="7">
         <v>10000</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="8">
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -513,19 +524,19 @@
       <c r="B3" s="3">
         <v>41731</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="5">
         <v>14</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="7">
-        <v>14</v>
-      </c>
-      <c r="F3" s="5">
+      <c r="F3" s="7">
         <v>112</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="7">
         <v>9.9</v>
       </c>
     </row>
@@ -536,17 +547,17 @@
       <c r="B4" s="3">
         <v>41773</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="5">
+      <c r="C4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="7">
         <v>34</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="7">
         <v>3.4</v>
       </c>
     </row>
@@ -555,128 +566,235 @@
         <v>4</v>
       </c>
       <c r="B5" s="3">
-        <v>41792</v>
-      </c>
-      <c r="C5" s="6" t="s">
+        <v>41791</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="7">
-        <v>200</v>
-      </c>
-      <c r="F5" s="5">
-        <v>5.77</v>
-      </c>
-      <c r="G5" s="5">
+      <c r="E5" s="5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="7">
+        <v>36</v>
+      </c>
+      <c r="G5" s="7">
         <v>9.9</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>41801</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="5">
-        <v>20</v>
-      </c>
-      <c r="G6" s="5"/>
+        <v>41792</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="5">
+        <v>200</v>
+      </c>
+      <c r="F6" s="7">
+        <v>5.77</v>
+      </c>
+      <c r="G6" s="7">
+        <v>9.9</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3">
-        <v>41890</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="5">
-        <v>1000.24</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>41801</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7">
+        <v>20</v>
+      </c>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3">
-        <v>370631</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="5">
-        <v>500</v>
-      </c>
-      <c r="G8" s="5"/>
+        <v>41890</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="7">
+        <v>1000.24</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B9" s="3">
-        <v>42083</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="7">
-        <v>14</v>
-      </c>
-      <c r="F9" s="5">
-        <v>239.15700000000001</v>
-      </c>
-      <c r="G9" s="5">
-        <v>9.9</v>
-      </c>
+        <v>370631</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7">
+        <v>500</v>
+      </c>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B10" s="3">
-        <v>42368</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="5">
-        <v>28.87</v>
-      </c>
-      <c r="G10" s="5"/>
+        <v>42083</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="5">
+        <v>18</v>
+      </c>
+      <c r="F10" s="7">
+        <v>239.15700000000001</v>
+      </c>
+      <c r="G10" s="7">
+        <v>9.9</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="3">
+        <v>42166</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7">
+        <v>40</v>
+      </c>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="3">
+        <v>42368</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="7">
+        <v>28.87</v>
+      </c>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B13" s="3">
+        <v>42402</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="7">
+        <v>-700</v>
+      </c>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3">
+        <v>42495</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="5">
+        <v>100</v>
+      </c>
+      <c r="F14" s="7">
+        <v>544</v>
+      </c>
+      <c r="G14" s="7">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="3">
+        <v>42532</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7">
+        <v>70</v>
+      </c>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="3">
         <v>42653</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="5">
-        <v>-700</v>
-      </c>
-      <c r="G11" s="5"/>
+      <c r="C16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="5">
+        <v>100</v>
+      </c>
+      <c r="F16" s="7">
+        <v>876</v>
+      </c>
+      <c r="G16" s="7">
+        <v>9.9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>